<commit_message>
rich dad name added
</commit_message>
<xml_diff>
--- a/metadata/ptsbook_data.xlsx
+++ b/metadata/ptsbook_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Free" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="72">
   <si>
     <t xml:space="preserve">Book Name</t>
   </si>
@@ -76,7 +76,169 @@
     <t xml:space="preserve">Pts#5</t>
   </si>
   <si>
-    <t xml:space="preserve">rich dad</t>
+    <t xml:space="preserve">பணக்கார அப்பா ஏழை அப்பா</t>
+  </si>
+  <si>
+    <t xml:space="preserve">أب غني أب فقير</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Богат татко беден татко</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ধনী বাবা দরিদ্র বাবা</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bogati tata jadni tata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ric pare, pobre pare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bohatý táta chudý táta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dad Rich Dad tlawd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rig far stakkels far</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reicher Vater, armer Vater</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Πλούσιος μπαμπάς φτωχός μπαμπάς</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Papa rico Papa pobre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rikas isa vaene isa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rikas isä köyhä isä</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mayaman na Tatay mahirap na tatay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Papa riche, papa pauvre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">શ્રીમંત પપ્પા ગરીબ પિતા</t>
+  </si>
+  <si>
+    <t xml:space="preserve">אבא עשיר אבא עני</t>
+  </si>
+  <si>
+    <t xml:space="preserve">धनी पिता गरीब पिता</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gazdag apa szegény apa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ayah kaya ayah malang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ríkur pabbi aumingja pabbi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Papà ricco papà povero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">金持ちのお父さんがかわいそうなお父さん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bapak-bapak ala bapak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ឪពុកកំសត់របស់ឪពុកអ្នកក្រ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ಶ್ರೀಮಂತ ತಂದೆ ಬಡ ಅಪ್ಪ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">부자 아빠 가난한 아빠</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bagāts tētis nabaga tētis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Turtingas tėtis vargšas tėtis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">സമ്പന്നമായ അച്ഛൻ ഡാഡ് ഡാഡി</t>
+  </si>
+  <si>
+    <t xml:space="preserve">श्रीमंत वडील गरीब बाबा</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ayah Ayah Kaya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rik pappa stakkars pappa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">धनी बुबा बुहारी</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rijke vader arme vader</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਅਮੀਰ ਪਿਤਾ ਮਾੜੇ ਡੈਡੀ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bogaty ojciec, biedny ojciec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pai rico Pai Pobre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tată bogat sărac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Богатый папа бедный папа</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ධනවත් තාත්තා දුප් තාත්තා</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bohatý otec chudobný otec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Babi i pasur baba i varfër</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Богати тата Јадник отац</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bapak beunghar bapak goréng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rik pappa stackars pappa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baba tajiri baba maskini</t>
+  </si>
+  <si>
+    <t xml:space="preserve">రిచ్ డాడ్ పేద తండ్రి</t>
+  </si>
+  <si>
+    <t xml:space="preserve">พ่อที่ร่ำรวย</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zengin Baba Fakir Baba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Багатий тато бідний тато</t>
+  </si>
+  <si>
+    <t xml:space="preserve">امیر والد غریب والد</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cha giàu có tội nghiệp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">有钱的爸爸爸爸</t>
   </si>
 </sst>
 </file>
@@ -88,7 +250,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -123,6 +285,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Noto Sans CJK SC"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -167,7 +334,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -200,6 +367,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -219,11 +390,11 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -372,7 +543,7 @@
       <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -672,7 +843,7 @@
       <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -862,27 +1033,320 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="57.35"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="0" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="0" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>17</v>
+      <c r="A3" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="8" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sample genner and aut added
</commit_message>
<xml_diff>
--- a/metadata/ptsbook_data.xlsx
+++ b/metadata/ptsbook_data.xlsx
@@ -5,13 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Free" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="education" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="fiction" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="book_name" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="author_name" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="gener_sheet" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="148">
   <si>
     <t xml:space="preserve">Book Name</t>
   </si>
@@ -239,6 +241,275 @@
   </si>
   <si>
     <t xml:space="preserve">有钱的爸爸爸爸</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ராபர்ட் கியோசாகி</t>
+  </si>
+  <si>
+    <t xml:space="preserve">روبرت كيوساكي</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Робърт Кийосаки</t>
+  </si>
+  <si>
+    <t xml:space="preserve">রবার্ট কিয়োসাকি</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robert Kiyosaki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">રોબર્ટ કિઓસાકી</t>
+  </si>
+  <si>
+    <t xml:space="preserve">רוברט קיוסאקי</t>
+  </si>
+  <si>
+    <t xml:space="preserve">रॉबर्ट कियोसाकी</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ロバート・キヨサキ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">រ៉ូប៊ឺតគីយូសាកូគី</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ರಾಬರ್ಟ್ ಕಿಯೋಸಾಕಿ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">로버트 키요 사키</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roberts Kiyosaki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robertas Kiyosaki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">റോബർട്ട് കിയോസാക്കി</t>
+  </si>
+  <si>
+    <t xml:space="preserve">रॉबर्ट किओसाकी</t>
+  </si>
+  <si>
+    <t xml:space="preserve">रोबर्ट क्यूसोस्की</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਰਾਬਰਟ ਕਿਯੋਸਾਕੀ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Роберт Кийосаки</t>
+  </si>
+  <si>
+    <t xml:space="preserve">රොබට් කියෝසකි</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Роберт Кииосаки</t>
+  </si>
+  <si>
+    <t xml:space="preserve">రాబర్ట్ కియోసాకి</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Роберт Кіясакі</t>
+  </si>
+  <si>
+    <t xml:space="preserve">رابرٹ کییوساکی</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">罗伯特</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">基亚萨基（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Robert Kiyosaki</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">）</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">education</t>
+  </si>
+  <si>
+    <t xml:space="preserve">கல்வி</t>
+  </si>
+  <si>
+    <t xml:space="preserve">تعليم</t>
+  </si>
+  <si>
+    <t xml:space="preserve">образование</t>
+  </si>
+  <si>
+    <t xml:space="preserve">শিক্ষা</t>
+  </si>
+  <si>
+    <t xml:space="preserve">obrazovanje</t>
+  </si>
+  <si>
+    <t xml:space="preserve">educació</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vzdělání</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addysg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uddannelse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ausbildung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">εκπαίδευση</t>
+  </si>
+  <si>
+    <t xml:space="preserve">educación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">haridus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">koulutus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edukasyon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">éducation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">શિક્ષણ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">חינוך</t>
+  </si>
+  <si>
+    <t xml:space="preserve">शिक्षा</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oktatás</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pendidikan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">menntun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">formazione scolastica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">教育</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pendhidhikan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ការអប់រម</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ಶಿಕ್ಷಣ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">교육</t>
+  </si>
+  <si>
+    <t xml:space="preserve">izglītība</t>
+  </si>
+  <si>
+    <t xml:space="preserve">išsilavinimas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">പഠനം</t>
+  </si>
+  <si>
+    <t xml:space="preserve">शिक्षण</t>
+  </si>
+  <si>
+    <t xml:space="preserve">utdanning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">onderwijs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਸਿੱਖਿਆ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edukacja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Educação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">educaţie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">අධ්යාපන</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vzdelávanie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arsim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">образовање</t>
+  </si>
+  <si>
+    <t xml:space="preserve">utbildning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elimu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">చదువు</t>
+  </si>
+  <si>
+    <t xml:space="preserve">การศึกษา</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eğitim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">освіта</t>
+  </si>
+  <si>
+    <t xml:space="preserve">تعلیم</t>
+  </si>
+  <si>
+    <t xml:space="preserve">giáo dục</t>
   </si>
 </sst>
 </file>
@@ -250,7 +521,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -283,6 +554,12 @@
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Noto Sans CJK SC"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -334,7 +611,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -371,6 +648,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,10 +672,10 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="A1:A61 B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -540,10 +821,10 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
+      <selection pane="topLeft" activeCell="G20" activeCellId="1" sqref="A1:A61 G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -840,10 +1121,10 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="1" sqref="A1:A61 G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1035,11 +1316,11 @@
   </sheetPr>
   <dimension ref="A1:A61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A1:A61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="57.35"/>
   </cols>
@@ -1347,6 +1628,664 @@
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="8" t="s">
         <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A61"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:A61"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A61"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:A61"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="9" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>